<commit_message>
Updated nets, added peak detector circuit into PCB schematic
</commit_message>
<xml_diff>
--- a/Hardware/Team02_EE209_BOM.xlsx
+++ b/Hardware/Team02_EE209_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Krithik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Krithik\Documents\GitHub\ee209-2020-project-team02\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429333E5-E7C3-43E4-9FAB-9F878274A94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC66A97-0ECA-4F19-BCE9-3EDAAAA3A866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1055,7 +1055,7 @@
   <dimension ref="A3:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated cf1 and cf2 to 4.7nF
</commit_message>
<xml_diff>
--- a/Hardware/Team02_EE209_BOM.xlsx
+++ b/Hardware/Team02_EE209_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Krithik\Documents\GitHub\ee209-2020-project-team02\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC66A97-0ECA-4F19-BCE9-3EDAAAA3A866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748CC333-DBEB-4654-AC19-C21D8CA3925A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,9 +279,6 @@
     <t>Cf1, Cf2</t>
   </si>
   <si>
-    <t>4n8</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>RP6</t>
+  </si>
+  <si>
+    <t>4n7</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,21 +1084,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
@@ -1564,10 +1564,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="B53" s="34" t="s">
-        <v>90</v>
       </c>
       <c r="C53" s="33">
         <v>5</v>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" s="33">
         <v>1</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" s="33">
         <v>1</v>
@@ -1629,7 +1629,7 @@
         <v>82</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C59" s="13">
         <v>8</v>
@@ -1640,7 +1640,7 @@
         <v>83</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C60" s="28">
         <v>2</v>
@@ -1648,19 +1648,14 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="B61" s="33" t="s">
-        <v>92</v>
-      </c>
       <c r="C61" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="14"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11"/>

</xml_diff>